<commit_message>
fixed the missing funtioanlity for mealplanner button
</commit_message>
<xml_diff>
--- a/build/app/intermediates/assets/debug/mergeDebugAssets/flutter_assets/assets/Recipe_table.xlsx
+++ b/build/app/intermediates/assets/debug/mergeDebugAssets/flutter_assets/assets/Recipe_table.xlsx
@@ -31,11 +31,11 @@
     <t>Vegan</t>
   </si>
   <si>
-    <t>1 ¼ cups all-purpose flour
+    <t>1 1/4 cups all-purpose flour
 2 tablespoons white sugar
-2 teaspoons baking powder
-½ teaspoon salt
-1 ¼ cups water
+2 tsp baking powder
+1/2 tsp salt
+1 1/4 cups water
 1 tablespoon oil</t>
   </si>
   <si>
@@ -55,13 +55,13 @@
 1 medium onion, chopped
 4 cloves garlic, minced
 1 small green bell pepper, diced
-1 (28 ounce) can diced tomatoes
-1 (16 ounce) can tomato sauce
-1 (6 ounce) can tomato paste
-2 teaspoons dried oregano
-2 teaspoons dried basil
-1 teaspoon salt
-½ teaspoon ground black pepper</t>
+1 can diced tomatoes
+1 can tomato sauce
+1 can tomato paste
+2 tsp dried oregano
+2 tsp dried basil
+1 tsp salt
+1/2 tsp ground black pepper</t>
   </si>
   <si>
     <t>Cook ground beef in a saucepan over medium-high heat with garlic, onion, and green pepper. Stir until the meat is brown and crumbly. The vegetables should be tender.
@@ -74,10 +74,10 @@
     <t>Vegetarian</t>
   </si>
   <si>
-    <t>3 large eggs (50 g each w/o shell)
-¼ tsp sugar
-¼ tsp Diamond Crystal kosher salt
-⅛ tsp freshly ground black pepper
+    <t>3 large eggs
+1/4 tsp sugar
+1/4 tsp Diamond Crystal kosher salt
+1/8 tsp freshly ground black pepper
 2 tsp milk
 2 Tbsp Japanese Kewpie mayonnaise
 4 slices shokupan (Japanese milk bread) 
@@ -99,8 +99,8 @@
 1 cup low fat shredded Colby Jack
 2 tbsp Half n Half
 2 tbsp reduced fat cream cheese
-¼ tsp garlic powder
-¼ tsp onion powder
+1/4 tsp garlic powder
+1/4 tsp onion powder
 14 tsp ground mustard</t>
   </si>
   <si>
@@ -120,8 +120,8 @@
   </si>
   <si>
     <t xml:space="preserve">skinless boneless chicken breasts 
-½ teaspoon salt 
-¼ teaspoon black pepper 
+1/2 tsp salt 
+1/4 tsp black pepper 
 2 tablespoons cooking fat </t>
   </si>
   <si>
@@ -134,19 +134,19 @@
     <t>Ratatouille</t>
   </si>
   <si>
-    <t>¼ cup coconut oil or extra-virgin olive oil
-¼ onion, finely chopped
+    <t>1/4 cup coconut oil or extra-virgin olive oil
+1/4 onion, finely chopped
 1 cup diced zucchini
 1 cup diced yellow squash
 1 cup diced eggplant
-½ teaspoon salt
-½ teaspoon black pepper
-½ cup finely diced green bell pepper
-½ cup finely diced red bell pepper
+1/2 teaspoon salt
+1/2 teaspoon black pepper
+1/2 cup finely diced green bell pepper
+1/2 cup finely diced red bell pepper
 2 cloves garlic, minced
 1 cup Tomato Sauce
 1 teaspoon balsamic vinegar
-3 fresh basil leaves, roughly chopped (optional)</t>
+3 fresh basil leaves, roughly chopped</t>
   </si>
   <si>
     <t>In a medium pot, heat the oil over medium heat, swirling to coat the bottom of the pot. When the oil is hot, add the onion and cook, stirring, until translucent, 2 to 3 minutes. 
@@ -163,13 +163,13 @@
     <t>Keto, Paleo</t>
   </si>
   <si>
-    <t xml:space="preserve">3 pounds (1.4 kg) chicken parts—legs, thighs, or breasts
-2 tablespoons (28 g) butter 
+    <t xml:space="preserve">3 pounds chicken parts—legs, thighs, or breasts
+2 tablespoons butter 
 1/2 medium onion, chopped 
-1/4 cup (60 ml) lemon juice 
+1/4 cup lemon juice 
 1/2 teaspoon chicken bouillon concentrate 
-1/4 cup (15 g) chopped fresh parsley 
-1 tablespoon (2 g) fresh thyme leaves </t>
+1/4 cup chopped fresh parsley 
+1 tablespoon fresh thyme leaves </t>
   </si>
   <si>
     <t xml:space="preserve">Cut the chicken into serving pieces and skin. In your big, heavy skillet, over medium heat, melt the butter and start the chicken browning. 

</xml_diff>